<commit_message>
3 New Regions (Development Levels)
</commit_message>
<xml_diff>
--- a/R/UI and SERVER/VERSION.1.1/Données/Geo/Regions/CRs/RDATA.CRs.xlsx
+++ b/R/UI and SERVER/VERSION.1.1/Données/Geo/Regions/CRs/RDATA.CRs.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">AFRICA</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;AFRICA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Africa&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;2&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;AFRICA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Africa&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;2</t>
   </si>
   <si>
     <t xml:space="preserve">#339900</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">ASIA</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;ASIA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Asia&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;142&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;ASIA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Asia&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;142</t>
   </si>
   <si>
     <t xml:space="preserve">#FF9900</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">EUROPE</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;EUROPE&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Europe&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;150&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;EUROPE&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Europe&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;150</t>
   </si>
   <si>
     <t xml:space="preserve">#003366</t>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Americas</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;LATIN AMERICA AND THE CARIBBEAN&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Americas&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;19&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;LATIN AMERICA AND THE CARIBBEAN&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Americas&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;19</t>
   </si>
   <si>
     <t xml:space="preserve">#FF0000</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">NORTHERN AMERICA</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;NORTHERN AMERICA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Americas&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;19&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;NORTHERN AMERICA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Americas&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;19</t>
   </si>
   <si>
     <t xml:space="preserve">#663399</t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">OCEANIA</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;OCEANIA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Oceania&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;9&lt;br&gt;</t>
+    <t xml:space="preserve">&lt;b&gt;Continental Region: &lt;/b&gt;OCEANIA&lt;br&gt;&lt;b&gt;Continent: &lt;/b&gt;Oceania&lt;br&gt;&lt;b&gt;M49 Code: &lt;/b&gt;9</t>
   </si>
   <si>
     <t xml:space="preserve">#FFCC00</t>

</xml_diff>